<commit_message>
Automating more of the decoding.
</commit_message>
<xml_diff>
--- a/ArduinoCoProcessor/CANBus/FRC_CAN/Extended Header Decoding.xlsx
+++ b/ArduinoCoProcessor/CANBus/FRC_CAN/Extended Header Decoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\GitHub\2024repo\ArduinoCoProcessor\CANBus\FRC_CAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B34407-F975-40FC-B7EE-FD7D6085D3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3691145-837F-4EB3-8117-0992D3EEAECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="2835" windowWidth="30780" windowHeight="15435" xr2:uid="{520C45A7-BD0F-47D4-A280-41EB6058BFAF}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{520C45A7-BD0F-47D4-A280-41EB6058BFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>0x01011840</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Robot Controller</t>
   </si>
   <si>
-    <t>0x061</t>
-  </si>
-  <si>
     <t>0x0A080040</t>
   </si>
   <si>
@@ -45,22 +42,10 @@
     <t>Team Use</t>
   </si>
   <si>
-    <t>0x001</t>
-  </si>
-  <si>
     <t>0x0A0848D1</t>
   </si>
   <si>
     <t>NI</t>
-  </si>
-  <si>
-    <t>Device = 0</t>
-  </si>
-  <si>
-    <t>0x123</t>
-  </si>
-  <si>
-    <t>Device = 17</t>
   </si>
   <si>
     <t>Device Types</t>
@@ -215,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +252,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F6F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,22 +435,28 @@
     <xf numFmtId="16" fontId="2" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,7 +779,7 @@
   <dimension ref="A1:AJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,215 +804,215 @@
     <row r="1" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
       <c r="AF2" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="AG2" s="7"/>
       <c r="AI2" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AJ2" s="7"/>
     </row>
     <row r="3" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
       <c r="AF3" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AG3" s="10">
         <v>0</v>
       </c>
       <c r="AI3" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="AJ3" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>28</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <f>B4-1</f>
         <v>27</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="14">
         <f t="shared" ref="D4:AD4" si="0">C4-1</f>
         <v>26</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="14">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="14">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="14">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="14">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="14">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="14">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="14">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="14">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="14">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="14">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="14">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="14">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="S4" s="16">
+      <c r="S4" s="14">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="T4" s="16">
+      <c r="T4" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="U4" s="16">
+      <c r="U4" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="V4" s="16">
+      <c r="V4" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="W4" s="16">
+      <c r="W4" s="14">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="X4" s="16">
+      <c r="X4" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Y4" s="16">
+      <c r="Y4" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="Z4" s="16">
+      <c r="Z4" s="14">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="AA4" s="16">
+      <c r="AA4" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AB4" s="16">
+      <c r="AB4" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="AC4" s="16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AD4" s="17">
+      <c r="AC4" s="14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD4" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1020,14 +1023,14 @@
         <v>1</v>
       </c>
       <c r="AI4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AJ4" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="str">
@@ -1147,73 +1150,75 @@
         <v>0</v>
       </c>
       <c r="AF5" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="AG5" s="10">
         <v>2</v>
       </c>
       <c r="AI5" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AJ5" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="21" t="str">
+        <f>"0x" &amp; DEC2HEX(X5+W5*2+V5*4+U5*8+T5*16+S5*32+R5*64+Q5*128+P5*256+O5*512, 3)</f>
+        <v>0x061</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="22" t="str">
+        <f>"Device = " &amp; AD5+AC5*2+AB5*4+AA5*8+Z5*16+Y5*32</f>
+        <v>Device = 0</v>
+      </c>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
       <c r="AF6" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AG6" s="11">
         <v>3</v>
       </c>
       <c r="AI6" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="AJ6" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>3</v>
+      <c r="A7" s="16" t="s">
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>MID(A7,3,1)</f>
@@ -1332,73 +1337,75 @@
         <v>0</v>
       </c>
       <c r="AF7" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="AG7" s="10">
         <v>4</v>
       </c>
       <c r="AI7" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="AJ7" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="21" t="str">
+        <f>"0x" &amp; DEC2HEX(X7+W7*2+V7*4+U7*8+T7*16+S7*32+R7*64+Q7*128+P7*256+O7*512, 3)</f>
+        <v>0x001</v>
+      </c>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="22" t="str">
+        <f>"Device = " &amp; AD7+AC7*2+AB7*4+AA7*8+Z7*16+Y7*32</f>
+        <v>Device = 0</v>
+      </c>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
       <c r="AF8" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AG8" s="11">
         <v>5</v>
       </c>
       <c r="AI8" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AJ8" s="11">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>7</v>
+      <c r="A9" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>MID(A9,3,1)</f>
@@ -1517,92 +1524,250 @@
         <v>1</v>
       </c>
       <c r="AF9" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="AG9" s="10">
         <v>6</v>
       </c>
       <c r="AI9" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="AJ9" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="21" t="str">
+        <f>"0x" &amp; DEC2HEX(X9+W9*2+V9*4+U9*8+T9*16+S9*32+R9*64+Q9*128+P9*256+O9*512, 3)</f>
+        <v>0x123</v>
+      </c>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="22" t="str">
+        <f>"Device = " &amp; AD9+AC9*2+AB9*4+AA9*8+Z9*16+Y9*32</f>
+        <v>Device = 17</v>
+      </c>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
       <c r="AF10" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="AG10" s="11">
         <v>7</v>
       </c>
       <c r="AI10" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AJ10" s="11">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="1" t="str">
+        <f>MID(A11,3,1)</f>
+        <v/>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>MID(HEX2BIN(MID($A11,4,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>MID(HEX2BIN(MID($A11,4,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f>MID(HEX2BIN(MID($A11,4,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f>MID(HEX2BIN(MID($A11,4,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,5,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,5,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,5,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,5,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,6,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,6,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,6,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <f>MID(HEX2BIN(MID($A11,6,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="6" t="str">
+        <f>MID(HEX2BIN(MID($A11,7,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="6" t="str">
+        <f>MID(HEX2BIN(MID($A11,7,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3" t="str">
+        <f>MID(HEX2BIN(MID($A11,7,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="3" t="str">
+        <f>MID(HEX2BIN(MID($A11,7,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="3" t="str">
+        <f>MID(HEX2BIN(MID($A11,8,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="3" t="str">
+        <f>MID(HEX2BIN(MID($A11,8,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="U11" s="4" t="str">
+        <f>MID(HEX2BIN(MID($A11,8,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="4" t="str">
+        <f>MID(HEX2BIN(MID($A11,8,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="4" t="str">
+        <f>MID(HEX2BIN(MID($A11,9,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="4" t="str">
+        <f>MID(HEX2BIN(MID($A11,9,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="5" t="str">
+        <f>MID(HEX2BIN(MID($A11,9,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="5" t="str">
+        <f>MID(HEX2BIN(MID($A11,9,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="5" t="str">
+        <f>MID(HEX2BIN(MID($A11,10,1), 4), 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="5" t="str">
+        <f>MID(HEX2BIN(MID($A11,10,1), 4), 2, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="5" t="str">
+        <f>MID(HEX2BIN(MID($A11,10,1), 4), 3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="5" t="str">
+        <f>MID(HEX2BIN(MID($A11,10,1), 4), 4, 1)</f>
+        <v>0</v>
+      </c>
       <c r="AF11" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AG11" s="10">
         <v>8</v>
       </c>
       <c r="AI11" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ11" s="10">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="21" t="str">
+        <f>"0x" &amp; DEC2HEX(X11+W11*2+V11*4+U11*8+T11*16+S11*32+R11*64+Q11*128+P11*256+O11*512, 3)</f>
+        <v>0x000</v>
+      </c>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="22" t="str">
+        <f>"Device = " &amp; AD11+AC11*2+AB11*4+AA11*8+Z11*16+Y11*32</f>
+        <v>Device = 0</v>
+      </c>
+      <c r="Z12" s="22"/>
+      <c r="AA12" s="22"/>
+      <c r="AB12" s="22"/>
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
       <c r="AF12" s="9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="AG12" s="11">
         <v>9</v>
       </c>
       <c r="AI12" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="AJ12" s="11">
         <v>9</v>
@@ -1610,13 +1775,13 @@
     </row>
     <row r="13" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AF13" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG13" s="10">
         <v>10</v>
       </c>
       <c r="AI13" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="AJ13" s="10">
         <v>10</v>
@@ -1624,13 +1789,13 @@
     </row>
     <row r="14" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AF14" s="9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="AG14" s="11">
         <v>11</v>
       </c>
       <c r="AI14" s="9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AJ14" s="11">
         <v>11</v>
@@ -1638,13 +1803,13 @@
     </row>
     <row r="15" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AF15" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="AG15" s="12">
         <v>45656</v>
       </c>
       <c r="AI15" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="AJ15" s="10">
         <v>12</v>
@@ -1652,13 +1817,13 @@
     </row>
     <row r="16" spans="1:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AF16" s="9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AG16" s="11">
         <v>31</v>
       </c>
       <c r="AI16" s="9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="AJ16" s="11">
         <v>13</v>
@@ -1666,7 +1831,7 @@
     </row>
     <row r="17" spans="35:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AI17" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="AJ17" s="10">
         <v>14</v>
@@ -1674,7 +1839,7 @@
     </row>
     <row r="18" spans="35:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AI18" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="AJ18" s="11">
         <v>15</v>
@@ -1682,7 +1847,7 @@
     </row>
     <row r="19" spans="35:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AI19" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AJ19" s="10">
         <v>16</v>
@@ -1690,25 +1855,18 @@
     </row>
     <row r="20" spans="35:36" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AI20" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="AJ20" s="11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="O2:X2"/>
-    <mergeCell ref="Y2:AD3"/>
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="G2:N3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="G6:N6"/>
-    <mergeCell ref="O6:X6"/>
-    <mergeCell ref="Y6:AD6"/>
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="U3:X3"/>
+  <mergeCells count="23">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="G12:N12"/>
+    <mergeCell ref="O12:X12"/>
+    <mergeCell ref="Y12:AD12"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="G10:N10"/>
     <mergeCell ref="O10:X10"/>
@@ -1717,6 +1875,17 @@
     <mergeCell ref="G8:N8"/>
     <mergeCell ref="O8:X8"/>
     <mergeCell ref="Y8:AD8"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G6:N6"/>
+    <mergeCell ref="O6:X6"/>
+    <mergeCell ref="Y6:AD6"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="U3:X3"/>
+    <mergeCell ref="O2:X2"/>
+    <mergeCell ref="Y2:AD3"/>
+    <mergeCell ref="B2:F3"/>
+    <mergeCell ref="G2:N3"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>